<commit_message>
Added mechanism to Close System 1 (web) and System 3 (desktop) applications. Retry mechanism created with 3 restarts for each transaction
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21727"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\srdjan.suc\Documents\UiPath\WI2ReFramework\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51F902B8-C08E-401F-8433-6D13A144E60A}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFD6EFC8-6E84-47FD-9AE5-2F7E5329F3DB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -569,7 +569,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z997"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
@@ -1686,8 +1686,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14:C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1738,7 +1738,7 @@
         <v>5</v>
       </c>
       <c r="B3">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C3" t="s">
         <v>6</v>

</xml_diff>